<commit_message>
Added stats and google DNS data.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scorpion\Documents\cse310\assignments\cse310_assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAAF1D35-2804-47DD-B9E2-1F2D6D407390}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205A7393-A061-4553-9080-8D8785498155}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5850" xr2:uid="{81C1206D-A8A0-4F44-8D13-8F81E0AE2C93}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>google.com</t>
   </si>
@@ -107,13 +107,25 @@
     <t>linkedin.com</t>
   </si>
   <si>
-    <t>Dig Results</t>
-  </si>
-  <si>
     <t>Trial</t>
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>local dns results</t>
+  </si>
+  <si>
+    <t>google dns results (8.8.8.8)</t>
+  </si>
+  <si>
+    <t>myDig.py Results</t>
+  </si>
+  <si>
+    <t>25th Percentile</t>
+  </si>
+  <si>
+    <t>75th Percentile</t>
   </si>
 </sst>
 </file>
@@ -465,22 +477,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B47C225-B6B1-4F5D-8BDE-030B0F9223E8}">
-  <dimension ref="B2:AA14"/>
+  <dimension ref="A2:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="12.578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -558,7 +571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>1</v>
       </c>
@@ -638,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>2</v>
       </c>
@@ -718,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>3</v>
       </c>
@@ -798,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
         <v>4</v>
       </c>
@@ -878,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>5</v>
       </c>
@@ -958,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1038,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1118,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1198,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1358,9 +1371,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <f>AVERAGE(C4:C13)</f>
@@ -1461,6 +1474,1866 @@
       <c r="AA14">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f>_xlfn.QUARTILE.INC(C$4:C$13,1 )</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:AA15" si="1">_xlfn.QUARTILE.INC(D$4:D$13,1 )</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <f>_xlfn.QUARTILE.INC(C$4:C$13,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:AA16" si="2">_xlfn.QUARTILE.INC(D$4:D$13,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S19" t="s">
+        <v>16</v>
+      </c>
+      <c r="T19" t="s">
+        <v>17</v>
+      </c>
+      <c r="U19" t="s">
+        <v>18</v>
+      </c>
+      <c r="V19" t="s">
+        <v>19</v>
+      </c>
+      <c r="W19" t="s">
+        <v>20</v>
+      </c>
+      <c r="X19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.105</v>
+      </c>
+      <c r="J20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K20">
+        <v>0.114</v>
+      </c>
+      <c r="L20">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="M20">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N20">
+        <v>0.104</v>
+      </c>
+      <c r="O20">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="P20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="R20">
+        <v>7.8E-2</v>
+      </c>
+      <c r="S20">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="T20">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="U20">
+        <v>0.1</v>
+      </c>
+      <c r="V20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="W20">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="X20">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="Y20">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="Z20">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="AA20">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <f>AVERAGE(C20:C29)</f>
+        <v>3.6999999999999997E-3</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:AA30" si="3">AVERAGE(D20:D29)</f>
+        <v>1.0199999999999999E-2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>1.0199999999999999E-2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>1.0199999999999999E-2</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>1.14E-2</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>1.03E-2</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>8.4000000000000012E-3</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="3"/>
+        <v>1.04E-2</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>1.0199999999999999E-2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="3"/>
+        <v>1.03E-2</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="3"/>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="3"/>
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="3"/>
+        <v>2.0300000000000002E-2</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="3"/>
+        <v>1.1600000000000001E-2</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="3"/>
+        <v>5.1299999999999998E-2</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="3"/>
+        <v>1.0100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>_xlfn.QUARTILE.INC(C20:C29,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:AA31" si="4">_xlfn.QUARTILE.INC(D20:D29,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>_xlfn.QUARTILE.INC(C20:C29, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:AA32" si="5">_xlfn.QUARTILE.INC(D20:D29, 3)</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" t="s">
+        <v>16</v>
+      </c>
+      <c r="T35" t="s">
+        <v>17</v>
+      </c>
+      <c r="U35" t="s">
+        <v>18</v>
+      </c>
+      <c r="V35" t="s">
+        <v>19</v>
+      </c>
+      <c r="W35" t="s">
+        <v>20</v>
+      </c>
+      <c r="X35" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" t="e">
+        <f>AVERAGE(C36:C45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" t="e">
+        <f t="shared" ref="D46" si="6">AVERAGE(D36:D45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" t="e">
+        <f t="shared" ref="E46" si="7">AVERAGE(E36:E45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" t="e">
+        <f t="shared" ref="F46" si="8">AVERAGE(F36:F45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" t="e">
+        <f t="shared" ref="G46" si="9">AVERAGE(G36:G45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" t="e">
+        <f t="shared" ref="H46" si="10">AVERAGE(H36:H45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" t="e">
+        <f t="shared" ref="I46" si="11">AVERAGE(I36:I45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" t="e">
+        <f t="shared" ref="J46" si="12">AVERAGE(J36:J45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" t="e">
+        <f t="shared" ref="K46" si="13">AVERAGE(K36:K45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" t="e">
+        <f t="shared" ref="L46" si="14">AVERAGE(L36:L45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" t="e">
+        <f t="shared" ref="M46" si="15">AVERAGE(M36:M45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N46" t="e">
+        <f t="shared" ref="N46" si="16">AVERAGE(N36:N45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O46" t="e">
+        <f t="shared" ref="O46" si="17">AVERAGE(O36:O45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P46" t="e">
+        <f t="shared" ref="P46" si="18">AVERAGE(P36:P45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q46" t="e">
+        <f t="shared" ref="Q46" si="19">AVERAGE(Q36:Q45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R46" t="e">
+        <f t="shared" ref="R46" si="20">AVERAGE(R36:R45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S46" t="e">
+        <f t="shared" ref="S46" si="21">AVERAGE(S36:S45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T46" t="e">
+        <f t="shared" ref="T46" si="22">AVERAGE(T36:T45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U46" t="e">
+        <f t="shared" ref="U46" si="23">AVERAGE(U36:U45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V46" t="e">
+        <f t="shared" ref="V46" si="24">AVERAGE(V36:V45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W46" t="e">
+        <f t="shared" ref="W46" si="25">AVERAGE(W36:W45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X46" t="e">
+        <f t="shared" ref="X46" si="26">AVERAGE(X36:X45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y46" t="e">
+        <f t="shared" ref="Y46" si="27">AVERAGE(Y36:Y45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z46" t="e">
+        <f t="shared" ref="Z46" si="28">AVERAGE(Z36:Z45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA46" t="e">
+        <f t="shared" ref="AA46" si="29">AVERAGE(AA36:AA45)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="e">
+        <f>_xlfn.QUARTILE.INC(C36:C45,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D47" t="e">
+        <f t="shared" ref="D47:AA47" si="30">_xlfn.QUARTILE.INC(D36:D45,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="I47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="R47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AA47" t="e">
+        <f t="shared" si="30"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="e">
+        <f>_xlfn.QUARTILE.INC(C36:C45, 3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D48" t="e">
+        <f t="shared" ref="D48:AA48" si="31">_xlfn.QUARTILE.INC(D36:D45, 3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="I48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="R48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AA48" t="e">
+        <f t="shared" si="31"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>